<commit_message>
I've uploaded a new PRD version with currections
</commit_message>
<xml_diff>
--- a/Articles/Articels index.xlsx
+++ b/Articles/Articels index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="8260" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve">EM segmentation </t>
+  </si>
+  <si>
+    <t>IsRelevant</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +132,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,6 +181,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +477,7 @@
     <col min="5" max="5" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -476,8 +493,11 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -489,8 +509,9 @@
         <v>6</v>
       </c>
       <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -500,8 +521,9 @@
         <v>7</v>
       </c>
       <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -511,8 +533,9 @@
         <v>8</v>
       </c>
       <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -520,8 +543,9 @@
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -529,8 +553,9 @@
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
       <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -538,8 +563,9 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -547,8 +573,9 @@
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -556,8 +583,9 @@
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -565,8 +593,9 @@
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -574,8 +603,9 @@
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -583,8 +613,9 @@
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -592,8 +623,9 @@
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -601,8 +633,9 @@
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -610,6 +643,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
       <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correction of the project number in the PDR
</commit_message>
<xml_diff>
--- a/Articles/Articels index.xlsx
+++ b/Articles/Articels index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -46,10 +46,6 @@
   <si>
     <t xml:space="preserve"> 
 J. Ashburner and K. Friston book, chapter 6: Segmentation</t>
-  </si>
-  <si>
-    <t>Segmenting mag- netic resonance (MR) images into different tissue classes, using a modified Gaussian mixture model.
-MOG - Mixture of Gaussians distribution model. This is parametric representations of image inten- sity distributions.</t>
   </si>
   <si>
     <t>Evaluation criteria: 
@@ -61,6 +57,17 @@
   </si>
   <si>
     <t>IsRelevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The article describes a MOG model with spatial priors (probabilities are vary over voxels). It also takes into considoration distoration and regularization (optimization of I voxals with k Geussians each).
+Segmenting magnetic resonance (MR) images into different tissue classes, using a modified Gaussian mixture model.
+MOG - Mixture of Gaussians distribution model. This is parametric representations of image intensity distributions.
+Loss function conssists of MOG parameters (meo,sigma,gama) , deforamtion (infectes the spatial priors - alpha), bias corrections (beta). Optimization using: EM for MOG parameters. LM for deforamation and bias.
+</t>
+  </si>
+  <si>
+    <t>a relevant youtube video list:
+https://www.youtube.com/watch?v=REypj2sy_5U&amp;index=1&amp;list=PLBv09BD7ez_4e9LtmK626Evn1ion6ynrt</t>
   </si>
 </sst>
 </file>
@@ -463,9 +470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="113" customHeight="1" x14ac:dyDescent="0.2">
@@ -506,9 +513,11 @@
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
@@ -518,7 +527,7 @@
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -530,7 +539,7 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>

</xml_diff>